<commit_message>
Updates for the Excel Version Control Tool
1. Change the location of the python file (Excel_diff.py) to the ./Scripts

2.Copy the necessary path to the ".gitattributes" and "config" file and remove the .gitattributes under "D_01_Excel_Version_Control_Tool"

3. Tested the version control tool under raven git repository.

4. Change the format of the Excel_diff.py to meet the requirements
</commit_message>
<xml_diff>
--- a/tests/reg_self_tests/D_01_Excel_Version_Control_Tool/01_version_control_tests.xlsx
+++ b/tests/reg_self_tests/D_01_Excel_Version_Control_Tool/01_version_control_tests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHENW\Box\WenChi.Cheng\05_Force_project\D_01_Excel_Version_Control_Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHENW\projects\raven\tests\reg_self_tests\D_01_Excel_Version_Control_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FDE354-69EF-47C4-8BDF-21BA63EEE660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF99EAC-AD2A-4126-9078-DEB29D93E1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="3090" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -254,38 +254,112 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right/>
+        <top style="medium">
+          <color theme="9"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="medium">
+          <color theme="9"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="9"/>
+        </left>
+        <right style="thin">
+          <color theme="9"/>
+        </right>
+        <top style="thin">
+          <color theme="9"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -431,80 +505,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="9"/>
-        </left>
-        <right/>
-        <top style="medium">
-          <color theme="9"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="medium">
-          <color theme="9"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="9"/>
-        </left>
-        <right style="thin">
-          <color theme="9"/>
-        </right>
-        <top style="thin">
-          <color theme="9"/>
-        </top>
-        <bottom style="thin">
-          <color theme="9"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -524,15 +524,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F350E51-C374-49CF-BA7F-C0F19F3EDB1F}" name="Inputs_table" displayName="Inputs_table" ref="A1:C8" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1F350E51-C374-49CF-BA7F-C0F19F3EDB1F}" name="Inputs_table" displayName="Inputs_table" ref="A1:C8" totalsRowShown="0" headerRowDxfId="7" tableBorderDxfId="6">
   <autoFilter ref="A1:C8" xr:uid="{1F350E51-C374-49CF-BA7F-C0F19F3EDB1F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A99731F4-5D6A-463E-A362-9B74946691C4}" name="Prameters" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{27F7C6B5-67C7-4BEA-ACA0-A4CA58085FCE}" name="Units " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{A99731F4-5D6A-463E-A362-9B74946691C4}" name="Prameters" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{27F7C6B5-67C7-4BEA-ACA0-A4CA58085FCE}" name="Units " dataDxfId="4"/>
     <tableColumn id="3" xr3:uid="{F107EC29-70F8-461B-9F30-30305269C175}" name="Value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
@@ -540,15 +540,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B29C5A0E-055B-4D93-BAA8-12F7D1C00A72}" name="Outputs_table" displayName="Outputs_table" ref="A2:C4" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B29C5A0E-055B-4D93-BAA8-12F7D1C00A72}" name="Outputs_table" displayName="Outputs_table" ref="A2:C4" totalsRowShown="0" headerRowDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A2:C4" xr:uid="{B29C5A0E-055B-4D93-BAA8-12F7D1C00A72}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1F5AC56E-DB8E-4FFF-AD0E-23109C2CE171}" name="Prameters" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A7AA723E-0BC8-4CC6-9FBD-28FF2B9C4BC9}" name="Units " dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{1F5AC56E-DB8E-4FFF-AD0E-23109C2CE171}" name="Prameters" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A7AA723E-0BC8-4CC6-9FBD-28FF2B9C4BC9}" name="Units " dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{9ECCDDA5-747B-4D72-B178-00429C01E917}" name="Value">
       <calculatedColumnFormula>Simluation_Tool_Example!B23</calculatedColumnFormula>
     </tableColumn>
@@ -823,7 +823,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -833,90 +833,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="19">
-        <v>400000000</v>
+      <c r="C2" s="18">
+        <v>100000000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>180000000</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>35000000</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="22">
+      <c r="C6" s="21">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="21">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="22">
         <v>0.1</v>
       </c>
     </row>
@@ -964,7 +964,7 @@
       </c>
       <c r="B2" s="2">
         <f>Inputs!C2</f>
-        <v>400000000</v>
+        <v>100000000</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -974,7 +974,7 @@
       </c>
       <c r="E2" s="3">
         <f>C2-B2</f>
-        <v>-400000000</v>
+        <v>-100000000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B23" s="6">
         <f>B2+NPV(Inputs!$C$8,B3:B22)</f>
-        <v>2230416199.7480898</v>
+        <v>1930416199.7480898</v>
       </c>
       <c r="C23" s="6">
         <f>C2+NPV(Inputs!$C$8,C3:C22)</f>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B24" s="7">
         <f>B23/D23</f>
-        <v>1.6614906767441548</v>
+        <v>1.4380134606624466</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1447,45 +1447,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <f>Simluation_Tool_Example!B23</f>
-        <v>2230416199.7480898</v>
+        <v>1930416199.7480898</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="17">
         <f>Simluation_Tool_Example!B24</f>
-        <v>1.6614906767441548</v>
+        <v>1.4380134606624466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporate comments from Paul on 3/15/2024
Address all the comments from Paul for "A few more minor changes". All the codes are tested before committing it through git.
</commit_message>
<xml_diff>
--- a/tests/reg_self_tests/D_01_Excel_Version_Control_Tool/01_version_control_tests.xlsx
+++ b/tests/reg_self_tests/D_01_Excel_Version_Control_Tool/01_version_control_tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHENW\projects\raven\tests\reg_self_tests\D_01_Excel_Version_Control_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF99EAC-AD2A-4126-9078-DEB29D93E1D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128AB74A-5C50-4C8C-9FFF-ABEBFCE6E33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="3090" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -851,7 +851,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="18">
-        <v>100000000</v>
+        <v>400000000</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -964,7 +964,7 @@
       </c>
       <c r="B2" s="2">
         <f>Inputs!C2</f>
-        <v>100000000</v>
+        <v>400000000</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -974,7 +974,7 @@
       </c>
       <c r="E2" s="3">
         <f>C2-B2</f>
-        <v>-100000000</v>
+        <v>-400000000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
@@ -1403,7 +1403,7 @@
       </c>
       <c r="B23" s="6">
         <f>B2+NPV(Inputs!$C$8,B3:B22)</f>
-        <v>1930416199.7480898</v>
+        <v>2230416199.7480898</v>
       </c>
       <c r="C23" s="6">
         <f>C2+NPV(Inputs!$C$8,C3:C22)</f>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B24" s="7">
         <f>B23/D23</f>
-        <v>1.4380134606624466</v>
+        <v>1.6614906767441548</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1473,7 +1473,7 @@
       </c>
       <c r="C3" s="12">
         <f>Simluation_Tool_Example!B23</f>
-        <v>1930416199.7480898</v>
+        <v>2230416199.7480898</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="C4" s="17">
         <f>Simluation_Tool_Example!B24</f>
-        <v>1.4380134606624466</v>
+        <v>1.6614906767441548</v>
       </c>
     </row>
   </sheetData>

</xml_diff>